<commit_message>
Save on new name
</commit_message>
<xml_diff>
--- a/templates/Test.xlsx
+++ b/templates/Test.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Lakštas1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="__sum__" vbProcedure="false">Lakštas1!$A$3:$C$4</definedName>
+    <definedName function="false" hidden="false" name="__sum__" vbProcedure="false">Lakštas1!$A$3:$D$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,9 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">Mokėtojas</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">Mokėtoja(s)</t>
   </si>
   <si>
     <t xml:space="preserve">Laikotarpis</t>
@@ -43,7 +43,13 @@
     <t xml:space="preserve">Vieneto kaina</t>
   </si>
   <si>
-    <t xml:space="preserve">Visa kaina</t>
+    <t xml:space="preserve">Parodymų skirtumas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suma, tenkanti mokėtojui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papildomi mokėjimai</t>
   </si>
   <si>
     <t xml:space="preserve">{{__service}}</t>
@@ -52,18 +58,25 @@
     <t xml:space="preserve">{{unit_price}}</t>
   </si>
   <si>
+    <t xml:space="preserve">{{diff}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{{price}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{additional_price}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-427];[RED]\-#,##0.00\ [$€-427]"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -93,6 +106,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -167,41 +188,61 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -219,6 +260,15 @@
     <cellStyle name="Suvestinės lentelės reikšmė" xfId="24"/>
     <cellStyle name="Suvestinės lentelės rezultatas" xfId="25"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -227,63 +277,112 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="15.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="4" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="G5" s="12" t="n">
+        <f aca="false">SUM($D$4:G4)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="12" t="n">
+        <f aca="false">SUM($E$4:H4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="G6" s="13" t="n">
+        <f aca="false">SUM(G5:H5)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G6:H6"/>
   </mergeCells>
+  <conditionalFormatting sqref="C1:C1048576 C3">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>-</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>